<commit_message>
Revamp landing page content and client logos
Updated the hero section with new messaging and featured players, expanded FAQ entries, and streamlined the client logos to use local images for Villarreal and Bayern Munich. Simplified the site header navigation and added a desktop menu. Removed unused sections from the marketing page. Added new signup data and images for client logos.
</commit_message>
<xml_diff>
--- a/data/signups.xlsx
+++ b/data/signups.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>timestamp</t>
   </si>
@@ -101,6 +101,39 @@
   </si>
   <si>
     <t>ads</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:41:16.912Z</t>
+  </si>
+  <si>
+    <t>jghnu67</t>
+  </si>
+  <si>
+    <t>hgju7</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>jghmuih</t>
+  </si>
+  <si>
+    <t>jmhkui6trfdd</t>
+  </si>
+  <si>
+    <t>hgngu@example.com</t>
+  </si>
+  <si>
+    <t>12306978493</t>
+  </si>
+  <si>
+    <t>stricker</t>
+  </si>
+  <si>
+    <t>7u7u7ijmhn</t>
+  </si>
+  <si>
+    <t>sumn</t>
   </si>
 </sst>
 </file>
@@ -487,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -640,6 +673,53 @@
         <v>29</v>
       </c>
     </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>